<commit_message>
Reporte de clientes con deuda
</commit_message>
<xml_diff>
--- a/reportes/base/ocierreVenta.xlsx
+++ b/reportes/base/ocierreVenta.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4003299a955809c3/Escritorio/calera/reportes/base/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uemar\Desktop\calera\report_sa_services\reportes\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="11_A3AD8052060DDFB58B4CFB36282AC21238724DF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E89CDA36-3D9B-4339-855A-121671A61160}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FF921A-1328-4B9B-A861-00246C0747BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Cierre de Ventas. </t>
   </si>
@@ -45,12 +57,15 @@
   <si>
     <t>Total ventas crédito</t>
   </si>
+  <si>
+    <t>Fecha:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +107,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aparajita"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -128,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -142,6 +163,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -458,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,51 +506,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" ht="10" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="F2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="9">
+        <f ca="1">TODAY()</f>
+        <v>44783</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="10" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -832,6 +865,15 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>